<commit_message>
Updated phylogenetic tree scripts
</commit_message>
<xml_diff>
--- a/Trees_WASTRAL/Data/names_dt1.xlsx
+++ b/Trees_WASTRAL/Data/names_dt1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.bitencourt/Documents/manuscripts/phylogenomics_Apocynaceae/Trees_WASTRAL/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/c.bitencourt/Documents/phylogenomics_Apocynaceae/Trees_WASTRAL/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66886186-6756-3C42-8B7E-D4D1288BA1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7978967-A5EC-E747-AA0B-E1025A067F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1600" windowWidth="29340" windowHeight="18880" xr2:uid="{265C166E-F460-404A-ADBF-A8385ED08C4C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29200" windowHeight="18880" xr2:uid="{265C166E-F460-404A-ADBF-A8385ED08C4C}"/>
   </bookViews>
   <sheets>
     <sheet name="names_dt1" sheetId="1" r:id="rId1"/>
@@ -1075,9 +1075,6 @@
     <t>Asclepiadoideae_Asclepiadeae_Metastelmatinae_Blepharodon_lineare_CB8</t>
   </si>
   <si>
-    <t>Asclepiadoideae_Asclepiadeae_Cynanchinae_Cynanchum_laeve_PAFTOL031815</t>
-  </si>
-  <si>
     <t>Asclepiadoideae_Asclepiadeae_Metastelmatinae_Ditassa_auriflora_CB95</t>
   </si>
   <si>
@@ -1315,9 +1312,6 @@
     <t>Asclepiadoideae_Asclepiadeae_Gonolobinae_Polystemma_scopulorum_PAFTOL031694</t>
   </si>
   <si>
-    <t>Asclepiadoideae_Asclepiadeae_Gonolobinae_Macroscepis_multiflora_PAFTOL031788</t>
-  </si>
-  <si>
     <t>Asclepiadoideae_Ceropegieae_Heterostemminae_Heterostemma_herbertii_PAFTOL031705</t>
   </si>
   <si>
@@ -1717,9 +1711,6 @@
     <t>apocynoids_Wrightieae_nosubtribe_Stephanostema_stenocarpum_PAFTOL005310</t>
   </si>
   <si>
-    <t>Asclepiadoideae_Asclepiadeae_Cynanchinae_Decanema_bojerianum_PAFTOL031789</t>
-  </si>
-  <si>
     <t>Asclepiadoideae_Ceropegieae_Stapeliinae_Piaranthus_geminatus_PAFTOL027291</t>
   </si>
   <si>
@@ -1969,9 +1960,6 @@
     <t>rauvolfioids_Aspidospermateae_nosubtribe_Aspidosperma_cylindrocarpon_PAFTOL004040</t>
   </si>
   <si>
-    <t>rauvolfioids_Aspidospermateae_nosubtribe_eissospermum_argenteum_PAFTOL025219</t>
-  </si>
-  <si>
     <t>rauvolfioids_Aspidospermateae_nosubtribe_Haplophyton_cimicidum_PAFTOL031732</t>
   </si>
   <si>
@@ -1982,6 +1970,18 @@
   </si>
   <si>
     <t>rauvolfioids_Aspidospermateae_nosubtribe_Vallesia_glabra_PAFTOL031744</t>
+  </si>
+  <si>
+    <t>Asclepiadoideae_Asclepiadeae_Cynanchinae_Cynanchum_luteifluens_PAFTOL031789</t>
+  </si>
+  <si>
+    <t>apocynoids_EOM_Prestoniinae_Prestonia_bahiensis_PAFTOL031788</t>
+  </si>
+  <si>
+    <t>Asclepiadoideae_Asclepiadeae_Gonolobinae_Chthamalia_producta_PAFTOL031815</t>
+  </si>
+  <si>
+    <t>rauvolfioids_Aspidospermateae_nosubtribe_Geissospermum_argenteum_PAFTOL025219</t>
   </si>
 </sst>
 </file>
@@ -2851,8 +2851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE674AB3-4F23-2841-AB42-B3E8C3FABEA2}">
   <dimension ref="A1:C326"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B319" sqref="B319:B326"/>
+    <sheetView tabSelected="1" topLeftCell="A234" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B254" sqref="B254"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2877,7 +2877,7 @@
         <v>293</v>
       </c>
       <c r="B2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C2">
         <v>277</v>
@@ -2888,7 +2888,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C3">
         <v>21</v>
@@ -2899,7 +2899,7 @@
         <v>336</v>
       </c>
       <c r="B4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C4">
         <v>317</v>
@@ -2910,7 +2910,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -2921,7 +2921,7 @@
         <v>63</v>
       </c>
       <c r="B6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C6">
         <v>60</v>
@@ -2932,7 +2932,7 @@
         <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C7">
         <v>169</v>
@@ -2943,7 +2943,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C8">
         <v>4</v>
@@ -2954,7 +2954,7 @@
         <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C9">
         <v>31</v>
@@ -2965,7 +2965,7 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C10">
         <v>104</v>
@@ -2976,7 +2976,7 @@
         <v>257</v>
       </c>
       <c r="B11" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C11">
         <v>243</v>
@@ -2987,7 +2987,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C12">
         <v>19</v>
@@ -2998,7 +2998,7 @@
         <v>228</v>
       </c>
       <c r="B13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C13">
         <v>216</v>
@@ -3009,7 +3009,7 @@
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C14">
         <v>32</v>
@@ -3020,7 +3020,7 @@
         <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C15">
         <v>82</v>
@@ -3031,7 +3031,7 @@
         <v>203</v>
       </c>
       <c r="B16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C16">
         <v>193</v>
@@ -3042,7 +3042,7 @@
         <v>214</v>
       </c>
       <c r="B17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C17">
         <v>203</v>
@@ -3053,7 +3053,7 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C18">
         <v>25</v>
@@ -3064,7 +3064,7 @@
         <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C19">
         <v>97</v>
@@ -3075,7 +3075,7 @@
         <v>323</v>
       </c>
       <c r="B20" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C20">
         <v>305</v>
@@ -3086,7 +3086,7 @@
         <v>144</v>
       </c>
       <c r="B21" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C21">
         <v>136</v>
@@ -3097,7 +3097,7 @@
         <v>158</v>
       </c>
       <c r="B22" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C22">
         <v>150</v>
@@ -3108,7 +3108,7 @@
         <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="C23">
         <v>74</v>
@@ -3119,7 +3119,7 @@
         <v>105</v>
       </c>
       <c r="B24" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C24">
         <v>100</v>
@@ -3130,7 +3130,7 @@
         <v>120</v>
       </c>
       <c r="B25" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C25">
         <v>114</v>
@@ -3141,7 +3141,7 @@
         <v>249</v>
       </c>
       <c r="B26" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C26">
         <v>236</v>
@@ -3152,7 +3152,7 @@
         <v>309</v>
       </c>
       <c r="B27" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C27">
         <v>292</v>
@@ -3163,7 +3163,7 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C28">
         <v>23</v>
@@ -3174,7 +3174,7 @@
         <v>322</v>
       </c>
       <c r="B29" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="C29">
         <v>304</v>
@@ -3185,7 +3185,7 @@
         <v>17</v>
       </c>
       <c r="B30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C30">
         <v>16</v>
@@ -3196,7 +3196,7 @@
         <v>233</v>
       </c>
       <c r="B31" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C31">
         <v>221</v>
@@ -3204,420 +3204,420 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>123</v>
+        <v>288</v>
       </c>
       <c r="B32" t="s">
-        <v>425</v>
+        <v>650</v>
       </c>
       <c r="C32">
-        <v>117</v>
+        <v>272</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C34">
-        <v>106</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C35">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C36">
-        <v>144</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>174</v>
+        <v>152</v>
       </c>
       <c r="B37" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C37">
-        <v>164</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>299</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C38">
-        <v>282</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>116</v>
+        <v>299</v>
       </c>
       <c r="B39" t="s">
-        <v>524</v>
+        <v>451</v>
       </c>
       <c r="C39">
-        <v>110</v>
+        <v>282</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C40">
-        <v>139</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>399</v>
+        <v>521</v>
       </c>
       <c r="C41">
-        <v>296</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>4</v>
+        <v>313</v>
       </c>
       <c r="B42" t="s">
-        <v>455</v>
+        <v>398</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>210</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C43">
-        <v>200</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>268</v>
+        <v>210</v>
       </c>
       <c r="B44" t="s">
-        <v>526</v>
+        <v>452</v>
       </c>
       <c r="C44">
-        <v>253</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>252</v>
+        <v>268</v>
       </c>
       <c r="B45" t="s">
-        <v>562</v>
+        <v>524</v>
       </c>
       <c r="C45">
-        <v>239</v>
+        <v>253</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>307</v>
+        <v>252</v>
       </c>
       <c r="B46" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C46">
-        <v>290</v>
+        <v>239</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>307</v>
       </c>
       <c r="B47" t="s">
-        <v>412</v>
+        <v>561</v>
       </c>
       <c r="C47">
-        <v>24</v>
+        <v>290</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B48" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C48">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>540</v>
+        <v>412</v>
       </c>
       <c r="C49">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C50">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="B51" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C51">
-        <v>67</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C52">
-        <v>109</v>
+        <v>67</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C53">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B54" t="s">
-        <v>414</v>
+        <v>542</v>
       </c>
       <c r="C54">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>172</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>545</v>
+        <v>413</v>
       </c>
       <c r="C55">
-        <v>162</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
       <c r="B56" t="s">
-        <v>415</v>
+        <v>543</v>
       </c>
       <c r="C56">
-        <v>186</v>
+        <v>162</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="B57" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C57">
-        <v>213</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="B58" t="s">
-        <v>546</v>
+        <v>415</v>
       </c>
       <c r="C58">
-        <v>218</v>
+        <v>213</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B59" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C59">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>284</v>
+        <v>239</v>
       </c>
       <c r="B60" t="s">
-        <v>417</v>
+        <v>545</v>
       </c>
       <c r="C60">
-        <v>268</v>
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B61" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C61">
-        <v>280</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B62" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C62">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B63" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C63">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>344</v>
+        <v>305</v>
       </c>
       <c r="B64" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C64">
-        <v>324</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B65" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C65">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>180</v>
+        <v>345</v>
       </c>
       <c r="B66" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C66">
-        <v>170</v>
+        <v>325</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>213</v>
+        <v>180</v>
       </c>
       <c r="B67" t="s">
-        <v>539</v>
+        <v>422</v>
       </c>
       <c r="C67">
-        <v>202</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>81</v>
+        <v>213</v>
       </c>
       <c r="B68" t="s">
-        <v>359</v>
+        <v>537</v>
       </c>
       <c r="C68">
-        <v>77</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="C69">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
@@ -3625,7 +3625,7 @@
         <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>564</v>
+        <v>649</v>
       </c>
       <c r="C70">
         <v>80</v>
@@ -3636,7 +3636,7 @@
         <v>285</v>
       </c>
       <c r="B71" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C71">
         <v>269</v>
@@ -3647,7 +3647,7 @@
         <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C72">
         <v>15</v>
@@ -3658,7 +3658,7 @@
         <v>62</v>
       </c>
       <c r="B73" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C73">
         <v>59</v>
@@ -3666,68 +3666,68 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
-        <v>551</v>
+        <v>651</v>
       </c>
       <c r="C74">
-        <v>71</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>426</v>
+        <v>549</v>
       </c>
       <c r="C75">
-        <v>112</v>
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B76" t="s">
-        <v>360</v>
+        <v>425</v>
       </c>
       <c r="C76">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B77" t="s">
-        <v>427</v>
+        <v>359</v>
       </c>
       <c r="C77">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>552</v>
+        <v>426</v>
       </c>
       <c r="C78">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>288</v>
+        <v>154</v>
       </c>
       <c r="B79" t="s">
-        <v>430</v>
+        <v>550</v>
       </c>
       <c r="C79">
-        <v>272</v>
+        <v>146</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
@@ -3735,7 +3735,7 @@
         <v>171</v>
       </c>
       <c r="B80" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C80">
         <v>161</v>
@@ -3746,7 +3746,7 @@
         <v>240</v>
       </c>
       <c r="B81" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C81">
         <v>227</v>
@@ -3757,7 +3757,7 @@
         <v>242</v>
       </c>
       <c r="B82" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C82">
         <v>229</v>
@@ -3768,7 +3768,7 @@
         <v>243</v>
       </c>
       <c r="B83" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C83">
         <v>230</v>
@@ -3779,7 +3779,7 @@
         <v>256</v>
       </c>
       <c r="B84" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C84">
         <v>242</v>
@@ -3790,7 +3790,7 @@
         <v>258</v>
       </c>
       <c r="B85" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C85">
         <v>244</v>
@@ -3801,7 +3801,7 @@
         <v>272</v>
       </c>
       <c r="B86" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C86">
         <v>257</v>
@@ -3812,7 +3812,7 @@
         <v>275</v>
       </c>
       <c r="B87" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C87">
         <v>260</v>
@@ -3823,7 +3823,7 @@
         <v>276</v>
       </c>
       <c r="B88" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C88">
         <v>261</v>
@@ -3834,7 +3834,7 @@
         <v>316</v>
       </c>
       <c r="B89" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C89">
         <v>298</v>
@@ -3845,7 +3845,7 @@
         <v>332</v>
       </c>
       <c r="B90" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C90">
         <v>314</v>
@@ -3889,7 +3889,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C94">
         <v>87</v>
@@ -3900,7 +3900,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C95">
         <v>88</v>
@@ -3911,7 +3911,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C96">
         <v>89</v>
@@ -3922,7 +3922,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C97">
         <v>90</v>
@@ -3933,7 +3933,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C98">
         <v>91</v>
@@ -3944,7 +3944,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C99">
         <v>92</v>
@@ -3955,7 +3955,7 @@
         <v>139</v>
       </c>
       <c r="B100" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C100">
         <v>131</v>
@@ -3966,7 +3966,7 @@
         <v>140</v>
       </c>
       <c r="B101" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C101">
         <v>132</v>
@@ -3977,7 +3977,7 @@
         <v>176</v>
       </c>
       <c r="B102" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C102">
         <v>166</v>
@@ -3988,7 +3988,7 @@
         <v>177</v>
       </c>
       <c r="B103" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C103">
         <v>167</v>
@@ -3999,7 +3999,7 @@
         <v>178</v>
       </c>
       <c r="B104" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C104">
         <v>168</v>
@@ -4010,7 +4010,7 @@
         <v>182</v>
       </c>
       <c r="B105" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C105">
         <v>172</v>
@@ -4021,7 +4021,7 @@
         <v>183</v>
       </c>
       <c r="B106" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C106">
         <v>173</v>
@@ -4032,7 +4032,7 @@
         <v>184</v>
       </c>
       <c r="B107" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C107">
         <v>174</v>
@@ -4043,7 +4043,7 @@
         <v>185</v>
       </c>
       <c r="B108" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C108">
         <v>175</v>
@@ -4054,7 +4054,7 @@
         <v>186</v>
       </c>
       <c r="B109" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C109">
         <v>176</v>
@@ -4065,7 +4065,7 @@
         <v>187</v>
       </c>
       <c r="B110" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C110">
         <v>177</v>
@@ -4076,7 +4076,7 @@
         <v>188</v>
       </c>
       <c r="B111" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C111">
         <v>178</v>
@@ -4087,7 +4087,7 @@
         <v>189</v>
       </c>
       <c r="B112" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C112">
         <v>179</v>
@@ -4098,7 +4098,7 @@
         <v>190</v>
       </c>
       <c r="B113" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C113">
         <v>180</v>
@@ -4109,7 +4109,7 @@
         <v>191</v>
       </c>
       <c r="B114" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C114">
         <v>181</v>
@@ -4120,7 +4120,7 @@
         <v>192</v>
       </c>
       <c r="B115" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C115">
         <v>182</v>
@@ -4131,7 +4131,7 @@
         <v>193</v>
       </c>
       <c r="B116" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C116">
         <v>183</v>
@@ -4142,7 +4142,7 @@
         <v>194</v>
       </c>
       <c r="B117" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C117">
         <v>184</v>
@@ -4153,7 +4153,7 @@
         <v>195</v>
       </c>
       <c r="B118" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C118">
         <v>185</v>
@@ -4164,7 +4164,7 @@
         <v>201</v>
       </c>
       <c r="B119" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C119">
         <v>191</v>
@@ -4175,7 +4175,7 @@
         <v>208</v>
       </c>
       <c r="B120" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C120">
         <v>198</v>
@@ -4186,7 +4186,7 @@
         <v>209</v>
       </c>
       <c r="B121" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C121">
         <v>199</v>
@@ -4197,7 +4197,7 @@
         <v>149</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C122">
         <v>141</v>
@@ -4208,7 +4208,7 @@
         <v>200</v>
       </c>
       <c r="B123" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C123">
         <v>190</v>
@@ -4219,7 +4219,7 @@
         <v>223</v>
       </c>
       <c r="B124" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C124">
         <v>211</v>
@@ -4230,7 +4230,7 @@
         <v>224</v>
       </c>
       <c r="B125" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C125">
         <v>212</v>
@@ -4241,7 +4241,7 @@
         <v>289</v>
       </c>
       <c r="B126" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C126">
         <v>273</v>
@@ -4252,7 +4252,7 @@
         <v>121</v>
       </c>
       <c r="B127" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C127">
         <v>115</v>
@@ -4263,7 +4263,7 @@
         <v>244</v>
       </c>
       <c r="B128" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C128">
         <v>231</v>
@@ -4274,7 +4274,7 @@
         <v>331</v>
       </c>
       <c r="B129" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="C129">
         <v>313</v>
@@ -4285,7 +4285,7 @@
         <v>232</v>
       </c>
       <c r="B130" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C130">
         <v>220</v>
@@ -4296,7 +4296,7 @@
         <v>320</v>
       </c>
       <c r="B131" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C131">
         <v>302</v>
@@ -4307,7 +4307,7 @@
         <v>325</v>
       </c>
       <c r="B132" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C132">
         <v>307</v>
@@ -4318,7 +4318,7 @@
         <v>235</v>
       </c>
       <c r="B133" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C133">
         <v>223</v>
@@ -4329,7 +4329,7 @@
         <v>19</v>
       </c>
       <c r="B134" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C134">
         <v>18</v>
@@ -4340,7 +4340,7 @@
         <v>107</v>
       </c>
       <c r="B135" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C135">
         <v>102</v>
@@ -4351,7 +4351,7 @@
         <v>207</v>
       </c>
       <c r="B136" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C136">
         <v>197</v>
@@ -4362,7 +4362,7 @@
         <v>274</v>
       </c>
       <c r="B137" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C137">
         <v>259</v>
@@ -4373,7 +4373,7 @@
         <v>294</v>
       </c>
       <c r="B138" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C138">
         <v>278</v>
@@ -4384,7 +4384,7 @@
         <v>141</v>
       </c>
       <c r="B139" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C139">
         <v>133</v>
@@ -4395,7 +4395,7 @@
         <v>70</v>
       </c>
       <c r="B140" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C140">
         <v>66</v>
@@ -4406,7 +4406,7 @@
         <v>162</v>
       </c>
       <c r="B141" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C141">
         <v>154</v>
@@ -4417,7 +4417,7 @@
         <v>220</v>
       </c>
       <c r="B142" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C142">
         <v>208</v>
@@ -4428,7 +4428,7 @@
         <v>234</v>
       </c>
       <c r="B143" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C143">
         <v>222</v>
@@ -4439,7 +4439,7 @@
         <v>24</v>
       </c>
       <c r="B144" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C144">
         <v>22</v>
@@ -4450,7 +4450,7 @@
         <v>32</v>
       </c>
       <c r="B145" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C145">
         <v>30</v>
@@ -4461,7 +4461,7 @@
         <v>39</v>
       </c>
       <c r="B146" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C146">
         <v>37</v>
@@ -4472,7 +4472,7 @@
         <v>50</v>
       </c>
       <c r="B147" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C147">
         <v>48</v>
@@ -4483,7 +4483,7 @@
         <v>56</v>
       </c>
       <c r="B148" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C148">
         <v>54</v>
@@ -4494,7 +4494,7 @@
         <v>85</v>
       </c>
       <c r="B149" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C149">
         <v>81</v>
@@ -4505,7 +4505,7 @@
         <v>99</v>
       </c>
       <c r="B150" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C150">
         <v>94</v>
@@ -4516,7 +4516,7 @@
         <v>100</v>
       </c>
       <c r="B151" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C151">
         <v>95</v>
@@ -4527,7 +4527,7 @@
         <v>101</v>
       </c>
       <c r="B152" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C152">
         <v>96</v>
@@ -4538,7 +4538,7 @@
         <v>104</v>
       </c>
       <c r="B153" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C153">
         <v>99</v>
@@ -4549,7 +4549,7 @@
         <v>143</v>
       </c>
       <c r="B154" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C154">
         <v>135</v>
@@ -4560,7 +4560,7 @@
         <v>157</v>
       </c>
       <c r="B155" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C155">
         <v>149</v>
@@ -4571,7 +4571,7 @@
         <v>159</v>
       </c>
       <c r="B156" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C156">
         <v>151</v>
@@ -4582,7 +4582,7 @@
         <v>199</v>
       </c>
       <c r="B157" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C157">
         <v>189</v>
@@ -4593,7 +4593,7 @@
         <v>215</v>
       </c>
       <c r="B158" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C158">
         <v>204</v>
@@ -4604,7 +4604,7 @@
         <v>218</v>
       </c>
       <c r="B159" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C159">
         <v>206</v>
@@ -4615,7 +4615,7 @@
         <v>231</v>
       </c>
       <c r="B160" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C160">
         <v>219</v>
@@ -4626,7 +4626,7 @@
         <v>247</v>
       </c>
       <c r="B161" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C161">
         <v>234</v>
@@ -4637,7 +4637,7 @@
         <v>259</v>
       </c>
       <c r="B162" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C162">
         <v>245</v>
@@ -4648,7 +4648,7 @@
         <v>260</v>
       </c>
       <c r="B163" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C163">
         <v>246</v>
@@ -4659,7 +4659,7 @@
         <v>265</v>
       </c>
       <c r="B164" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C164">
         <v>250</v>
@@ -4670,7 +4670,7 @@
         <v>271</v>
       </c>
       <c r="B165" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C165">
         <v>256</v>
@@ -4681,7 +4681,7 @@
         <v>273</v>
       </c>
       <c r="B166" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C166">
         <v>258</v>
@@ -4692,7 +4692,7 @@
         <v>295</v>
       </c>
       <c r="B167" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C167">
         <v>279</v>
@@ -4703,7 +4703,7 @@
         <v>302</v>
       </c>
       <c r="B168" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C168">
         <v>285</v>
@@ -4714,7 +4714,7 @@
         <v>303</v>
       </c>
       <c r="B169" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C169">
         <v>286</v>
@@ -4725,7 +4725,7 @@
         <v>321</v>
       </c>
       <c r="B170" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C170">
         <v>303</v>
@@ -4736,7 +4736,7 @@
         <v>329</v>
       </c>
       <c r="B171" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C171">
         <v>311</v>
@@ -4747,7 +4747,7 @@
         <v>330</v>
       </c>
       <c r="B172" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C172">
         <v>312</v>
@@ -4758,7 +4758,7 @@
         <v>106</v>
       </c>
       <c r="B173" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C173">
         <v>101</v>
@@ -4769,7 +4769,7 @@
         <v>112</v>
       </c>
       <c r="B174" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C174">
         <v>107</v>
@@ -4780,7 +4780,7 @@
         <v>64</v>
       </c>
       <c r="B175" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C175">
         <v>61</v>
@@ -4791,7 +4791,7 @@
         <v>119</v>
       </c>
       <c r="B176" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C176">
         <v>113</v>
@@ -4802,7 +4802,7 @@
         <v>18</v>
       </c>
       <c r="B177" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C177">
         <v>17</v>
@@ -4813,7 +4813,7 @@
         <v>48</v>
       </c>
       <c r="B178" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="C178">
         <v>46</v>
@@ -4824,7 +4824,7 @@
         <v>65</v>
       </c>
       <c r="B179" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C179">
         <v>62</v>
@@ -4835,7 +4835,7 @@
         <v>72</v>
       </c>
       <c r="B180" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C180">
         <v>68</v>
@@ -4846,7 +4846,7 @@
         <v>83</v>
       </c>
       <c r="B181" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C181">
         <v>79</v>
@@ -4857,7 +4857,7 @@
         <v>90</v>
       </c>
       <c r="B182" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="C182">
         <v>85</v>
@@ -4868,7 +4868,7 @@
         <v>91</v>
       </c>
       <c r="B183" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C183">
         <v>86</v>
@@ -4879,7 +4879,7 @@
         <v>98</v>
       </c>
       <c r="B184" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C184">
         <v>93</v>
@@ -4890,7 +4890,7 @@
         <v>131</v>
       </c>
       <c r="B185" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C185">
         <v>123</v>
@@ -4901,7 +4901,7 @@
         <v>135</v>
       </c>
       <c r="B186" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C186">
         <v>127</v>
@@ -4912,7 +4912,7 @@
         <v>138</v>
       </c>
       <c r="B187" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C187">
         <v>130</v>
@@ -4923,7 +4923,7 @@
         <v>148</v>
       </c>
       <c r="B188" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C188">
         <v>140</v>
@@ -4934,7 +4934,7 @@
         <v>166</v>
       </c>
       <c r="B189" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C189">
         <v>157</v>
@@ -4945,7 +4945,7 @@
         <v>173</v>
       </c>
       <c r="B190" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C190">
         <v>163</v>
@@ -4956,7 +4956,7 @@
         <v>219</v>
       </c>
       <c r="B191" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C191">
         <v>207</v>
@@ -4967,7 +4967,7 @@
         <v>227</v>
       </c>
       <c r="B192" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C192">
         <v>215</v>
@@ -4978,7 +4978,7 @@
         <v>264</v>
       </c>
       <c r="B193" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C193">
         <v>249</v>
@@ -4989,7 +4989,7 @@
         <v>270</v>
       </c>
       <c r="B194" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C194">
         <v>255</v>
@@ -5000,7 +5000,7 @@
         <v>277</v>
       </c>
       <c r="B195" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="C195">
         <v>262</v>
@@ -5011,7 +5011,7 @@
         <v>280</v>
       </c>
       <c r="B196" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="C196">
         <v>265</v>
@@ -5022,7 +5022,7 @@
         <v>292</v>
       </c>
       <c r="B197" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C197">
         <v>276</v>
@@ -5033,7 +5033,7 @@
         <v>308</v>
       </c>
       <c r="B198" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C198">
         <v>291</v>
@@ -5044,7 +5044,7 @@
         <v>327</v>
       </c>
       <c r="B199" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="C199">
         <v>309</v>
@@ -5055,7 +5055,7 @@
         <v>342</v>
       </c>
       <c r="B200" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C200">
         <v>322</v>
@@ -5187,7 +5187,7 @@
         <v>31</v>
       </c>
       <c r="B212" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="C212">
         <v>29</v>
@@ -5198,7 +5198,7 @@
         <v>36</v>
       </c>
       <c r="B213" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C213">
         <v>34</v>
@@ -5209,7 +5209,7 @@
         <v>37</v>
       </c>
       <c r="B214" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="C214">
         <v>35</v>
@@ -5220,7 +5220,7 @@
         <v>38</v>
       </c>
       <c r="B215" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C215">
         <v>36</v>
@@ -5231,7 +5231,7 @@
         <v>43</v>
       </c>
       <c r="B216" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="C216">
         <v>41</v>
@@ -5242,7 +5242,7 @@
         <v>49</v>
       </c>
       <c r="B217" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C217">
         <v>47</v>
@@ -5253,7 +5253,7 @@
         <v>61</v>
       </c>
       <c r="B218" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C218">
         <v>58</v>
@@ -5264,7 +5264,7 @@
         <v>76</v>
       </c>
       <c r="B219" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="C219">
         <v>72</v>
@@ -5275,7 +5275,7 @@
         <v>77</v>
       </c>
       <c r="B220" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C220">
         <v>73</v>
@@ -5286,7 +5286,7 @@
         <v>103</v>
       </c>
       <c r="B221" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C221">
         <v>98</v>
@@ -5297,7 +5297,7 @@
         <v>110</v>
       </c>
       <c r="B222" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C222">
         <v>105</v>
@@ -5308,7 +5308,7 @@
         <v>117</v>
       </c>
       <c r="B223" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C223">
         <v>111</v>
@@ -5319,7 +5319,7 @@
         <v>146</v>
       </c>
       <c r="B224" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C224">
         <v>138</v>
@@ -5330,7 +5330,7 @@
         <v>167</v>
       </c>
       <c r="B225" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C225">
         <v>158</v>
@@ -5341,7 +5341,7 @@
         <v>198</v>
       </c>
       <c r="B226" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C226">
         <v>188</v>
@@ -5352,7 +5352,7 @@
         <v>205</v>
       </c>
       <c r="B227" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C227">
         <v>195</v>
@@ -5363,7 +5363,7 @@
         <v>236</v>
       </c>
       <c r="B228" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C228">
         <v>224</v>
@@ -5374,7 +5374,7 @@
         <v>245</v>
       </c>
       <c r="B229" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C229">
         <v>232</v>
@@ -5385,7 +5385,7 @@
         <v>246</v>
       </c>
       <c r="B230" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="C230">
         <v>233</v>
@@ -5396,7 +5396,7 @@
         <v>266</v>
       </c>
       <c r="B231" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="C231">
         <v>251</v>
@@ -5407,7 +5407,7 @@
         <v>279</v>
       </c>
       <c r="B232" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C232">
         <v>264</v>
@@ -5418,7 +5418,7 @@
         <v>281</v>
       </c>
       <c r="B233" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="C233">
         <v>266</v>
@@ -5429,7 +5429,7 @@
         <v>287</v>
       </c>
       <c r="B234" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C234">
         <v>271</v>
@@ -5440,7 +5440,7 @@
         <v>310</v>
       </c>
       <c r="B235" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C235">
         <v>293</v>
@@ -5451,7 +5451,7 @@
         <v>312</v>
       </c>
       <c r="B236" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C236">
         <v>295</v>
@@ -5462,7 +5462,7 @@
         <v>319</v>
       </c>
       <c r="B237" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C237">
         <v>301</v>
@@ -5473,7 +5473,7 @@
         <v>7</v>
       </c>
       <c r="B238" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C238">
         <v>6</v>
@@ -5484,7 +5484,7 @@
         <v>8</v>
       </c>
       <c r="B239" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C239">
         <v>7</v>
@@ -5495,7 +5495,7 @@
         <v>9</v>
       </c>
       <c r="B240" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="C240">
         <v>8</v>
@@ -5506,7 +5506,7 @@
         <v>10</v>
       </c>
       <c r="B241" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C241">
         <v>9</v>
@@ -5517,7 +5517,7 @@
         <v>160</v>
       </c>
       <c r="B242" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C242">
         <v>152</v>
@@ -5528,7 +5528,7 @@
         <v>161</v>
       </c>
       <c r="B243" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C243">
         <v>153</v>
@@ -5539,7 +5539,7 @@
         <v>263</v>
       </c>
       <c r="B244" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C244">
         <v>248</v>
@@ -5550,7 +5550,7 @@
         <v>58</v>
       </c>
       <c r="B245" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C245">
         <v>56</v>
@@ -5561,7 +5561,7 @@
         <v>69</v>
       </c>
       <c r="B246" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C246">
         <v>65</v>
@@ -5572,7 +5572,7 @@
         <v>250</v>
       </c>
       <c r="B247" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C247">
         <v>237</v>
@@ -5583,7 +5583,7 @@
         <v>13</v>
       </c>
       <c r="B248" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C248">
         <v>12</v>
@@ -5594,7 +5594,7 @@
         <v>30</v>
       </c>
       <c r="B249" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="C249">
         <v>28</v>
@@ -5605,7 +5605,7 @@
         <v>124</v>
       </c>
       <c r="B250" t="s">
-        <v>648</v>
+        <v>652</v>
       </c>
       <c r="C250">
         <v>118</v>
@@ -5616,7 +5616,7 @@
         <v>137</v>
       </c>
       <c r="B251" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="C251">
         <v>129</v>
@@ -5627,7 +5627,7 @@
         <v>181</v>
       </c>
       <c r="B252" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="C252">
         <v>171</v>
@@ -5638,7 +5638,7 @@
         <v>311</v>
       </c>
       <c r="B253" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="C253">
         <v>294</v>
@@ -5649,7 +5649,7 @@
         <v>337</v>
       </c>
       <c r="B254" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="C254">
         <v>318</v>
@@ -5660,7 +5660,7 @@
         <v>2</v>
       </c>
       <c r="B255" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C255">
         <v>1</v>
@@ -5671,7 +5671,7 @@
         <v>3</v>
       </c>
       <c r="B256" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C256">
         <v>2</v>
@@ -5682,7 +5682,7 @@
         <v>51</v>
       </c>
       <c r="B257" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C257">
         <v>49</v>
@@ -5693,7 +5693,7 @@
         <v>52</v>
       </c>
       <c r="B258" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C258">
         <v>50</v>
@@ -5704,7 +5704,7 @@
         <v>132</v>
       </c>
       <c r="B259" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="C259">
         <v>124</v>
@@ -5715,7 +5715,7 @@
         <v>248</v>
       </c>
       <c r="B260" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="C260">
         <v>235</v>
@@ -5726,7 +5726,7 @@
         <v>251</v>
       </c>
       <c r="B261" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="C261">
         <v>238</v>
@@ -5737,7 +5737,7 @@
         <v>175</v>
       </c>
       <c r="B262" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C262">
         <v>165</v>
@@ -5748,7 +5748,7 @@
         <v>306</v>
       </c>
       <c r="B263" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
       <c r="C263">
         <v>289</v>
@@ -5759,7 +5759,7 @@
         <v>142</v>
       </c>
       <c r="B264" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C264">
         <v>134</v>
@@ -5770,7 +5770,7 @@
         <v>202</v>
       </c>
       <c r="B265" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C265">
         <v>192</v>
@@ -5781,7 +5781,7 @@
         <v>255</v>
       </c>
       <c r="B266" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C266">
         <v>241</v>
@@ -5792,7 +5792,7 @@
         <v>15</v>
       </c>
       <c r="B267" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C267">
         <v>14</v>
@@ -5803,7 +5803,7 @@
         <v>54</v>
       </c>
       <c r="B268" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C268">
         <v>52</v>
@@ -5814,7 +5814,7 @@
         <v>55</v>
       </c>
       <c r="B269" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C269">
         <v>53</v>
@@ -5825,7 +5825,7 @@
         <v>324</v>
       </c>
       <c r="B270" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C270">
         <v>306</v>
@@ -5836,7 +5836,7 @@
         <v>12</v>
       </c>
       <c r="B271" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C271">
         <v>11</v>
@@ -5847,7 +5847,7 @@
         <v>168</v>
       </c>
       <c r="B272" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C272">
         <v>159</v>
@@ -5858,7 +5858,7 @@
         <v>197</v>
       </c>
       <c r="B273" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C273">
         <v>187</v>
@@ -5869,7 +5869,7 @@
         <v>204</v>
       </c>
       <c r="B274" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C274">
         <v>194</v>
@@ -5880,7 +5880,7 @@
         <v>206</v>
       </c>
       <c r="B275" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C275">
         <v>196</v>
@@ -5891,7 +5891,7 @@
         <v>269</v>
       </c>
       <c r="B276" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C276">
         <v>254</v>
@@ -5902,7 +5902,7 @@
         <v>300</v>
       </c>
       <c r="B277" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C277">
         <v>283</v>
@@ -5913,7 +5913,7 @@
         <v>301</v>
       </c>
       <c r="B278" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C278">
         <v>284</v>
@@ -5924,7 +5924,7 @@
         <v>45</v>
       </c>
       <c r="B279" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C279">
         <v>43</v>
@@ -5935,7 +5935,7 @@
         <v>46</v>
       </c>
       <c r="B280" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="C280">
         <v>44</v>
@@ -5946,7 +5946,7 @@
         <v>53</v>
       </c>
       <c r="B281" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C281">
         <v>51</v>
@@ -5957,7 +5957,7 @@
         <v>74</v>
       </c>
       <c r="B282" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="C282">
         <v>70</v>
@@ -5968,7 +5968,7 @@
         <v>108</v>
       </c>
       <c r="B283" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="C283">
         <v>103</v>
@@ -5979,7 +5979,7 @@
         <v>286</v>
       </c>
       <c r="B284" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C284">
         <v>270</v>
@@ -5990,7 +5990,7 @@
         <v>317</v>
       </c>
       <c r="B285" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C285">
         <v>299</v>
@@ -6001,7 +6001,7 @@
         <v>318</v>
       </c>
       <c r="B286" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C286">
         <v>300</v>
@@ -6012,7 +6012,7 @@
         <v>339</v>
       </c>
       <c r="B287" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C287">
         <v>320</v>
@@ -6023,7 +6023,7 @@
         <v>150</v>
       </c>
       <c r="B288" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C288">
         <v>142</v>
@@ -6034,7 +6034,7 @@
         <v>153</v>
       </c>
       <c r="B289" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C289">
         <v>145</v>
@@ -6045,7 +6045,7 @@
         <v>267</v>
       </c>
       <c r="B290" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C290">
         <v>252</v>
@@ -6056,7 +6056,7 @@
         <v>338</v>
       </c>
       <c r="B291" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C291">
         <v>319</v>
@@ -6067,7 +6067,7 @@
         <v>73</v>
       </c>
       <c r="B292" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C292">
         <v>69</v>
@@ -6078,7 +6078,7 @@
         <v>136</v>
       </c>
       <c r="B293" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C293">
         <v>128</v>
@@ -6089,7 +6089,7 @@
         <v>155</v>
       </c>
       <c r="B294" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C294">
         <v>147</v>
@@ -6100,7 +6100,7 @@
         <v>229</v>
       </c>
       <c r="B295" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C295">
         <v>217</v>
@@ -6111,7 +6111,7 @@
         <v>14</v>
       </c>
       <c r="B296" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C296">
         <v>13</v>
@@ -6122,7 +6122,7 @@
         <v>57</v>
       </c>
       <c r="B297" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C297">
         <v>55</v>
@@ -6133,7 +6133,7 @@
         <v>66</v>
       </c>
       <c r="B298" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C298">
         <v>63</v>
@@ -6144,7 +6144,7 @@
         <v>80</v>
       </c>
       <c r="B299" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C299">
         <v>76</v>
@@ -6155,7 +6155,7 @@
         <v>87</v>
       </c>
       <c r="B300" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C300">
         <v>83</v>
@@ -6166,7 +6166,7 @@
         <v>156</v>
       </c>
       <c r="B301" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C301">
         <v>148</v>
@@ -6177,7 +6177,7 @@
         <v>221</v>
       </c>
       <c r="B302" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C302">
         <v>209</v>
@@ -6188,7 +6188,7 @@
         <v>222</v>
       </c>
       <c r="B303" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C303">
         <v>210</v>
@@ -6199,7 +6199,7 @@
         <v>226</v>
       </c>
       <c r="B304" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C304">
         <v>214</v>
@@ -6210,7 +6210,7 @@
         <v>278</v>
       </c>
       <c r="B305" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C305">
         <v>263</v>
@@ -6221,7 +6221,7 @@
         <v>335</v>
       </c>
       <c r="B306" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C306">
         <v>316</v>
@@ -6232,7 +6232,7 @@
         <v>42</v>
       </c>
       <c r="B307" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="C307">
         <v>40</v>
@@ -6243,7 +6243,7 @@
         <v>79</v>
       </c>
       <c r="B308" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C308">
         <v>75</v>
@@ -6254,7 +6254,7 @@
         <v>163</v>
       </c>
       <c r="B309" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="C309">
         <v>155</v>
@@ -6265,7 +6265,7 @@
         <v>343</v>
       </c>
       <c r="B310" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C310">
         <v>323</v>
@@ -6364,7 +6364,7 @@
         <v>47</v>
       </c>
       <c r="B319" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C319">
         <v>45</v>
@@ -6375,7 +6375,7 @@
         <v>127</v>
       </c>
       <c r="B320" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C320">
         <v>120</v>
@@ -6386,7 +6386,7 @@
         <v>133</v>
       </c>
       <c r="B321" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C321">
         <v>125</v>
@@ -6397,7 +6397,7 @@
         <v>241</v>
       </c>
       <c r="B322" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C322">
         <v>228</v>
@@ -6408,7 +6408,7 @@
         <v>290</v>
       </c>
       <c r="B323" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C323">
         <v>274</v>
@@ -6419,7 +6419,7 @@
         <v>291</v>
       </c>
       <c r="B324" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="C324">
         <v>275</v>
@@ -6430,7 +6430,7 @@
         <v>326</v>
       </c>
       <c r="B325" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="C325">
         <v>308</v>
@@ -6441,7 +6441,7 @@
         <v>328</v>
       </c>
       <c r="B326" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C326">
         <v>310</v>

</xml_diff>